<commit_message>
update reject and accept files
</commit_message>
<xml_diff>
--- a/Assignment Details.xlsx
+++ b/Assignment Details.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23260" yWindow="460" windowWidth="10000" windowHeight="19700" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="24900" yWindow="520" windowWidth="10000" windowHeight="19700" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blocked Users" sheetId="2" r:id="rId2"/>
+    <sheet name="Blocked and white listed users" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="119">
   <si>
     <t>Query</t>
   </si>
@@ -175,13 +176,223 @@
   </si>
   <si>
     <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0006wb-17-18108;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0700wb-82-24900;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>A1XZTIJD9WBHLJ</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0612wb-77-22720;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1010wb-28-23486;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1400wb-72-33205;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>A21I4DTJGWJYQJ</t>
+  </si>
+  <si>
+    <t>White List</t>
+  </si>
+  <si>
+    <t>A23CV5SKZAJHQJ</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0701wb-34-09751;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0701wb-77-18683;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>A2XYDJS33I2341</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1803wb-09-05486;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1019wb-59-10540;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0510wb-19-10077;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>A33MF851P56BFH</t>
+  </si>
+  <si>
+    <t>A39N0WW02VT0MB</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1501wb-89-30611;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0004wb-90-16571;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1512wb-68-00783;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0100tw-25-07072;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>AZZM966F90AL1</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0108wb-76-34619;topicId=2s7f67</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0206wb-15-16411;topicId=36e8h1</t>
+  </si>
+  <si>
+    <t>A1IHI23KH87K5W</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0509wb-15-11462;topicId=36e8h1</t>
+  </si>
+  <si>
+    <t>Dodgy</t>
+  </si>
+  <si>
+    <t>A1T79J0XQXDDGC</t>
+  </si>
+  <si>
+    <t>A1XC5OV00MECKQ</t>
+  </si>
+  <si>
+    <t>A2IG18D6M0GNUZ</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1910wb-88-29811;topicId=36e8h1</t>
+  </si>
+  <si>
+    <t>A33D8QFFK8WBTQ</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1009wb-12-29554;topicId=36e8h1</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1009wb-05-08779;topicId=36e8h1</t>
+  </si>
+  <si>
+    <t>A3B67I3A0YR2D</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0103wb-29-09191;topicId=36e8h1</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0910wb-27-05473;topicId=2trr62</t>
+  </si>
+  <si>
+    <t>A1PLY1H54IPJRB</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0212wb-00-30776;topicId=2trr62</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1607wb-47-19368;topicId=2trr62</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0210wb-55-25590;topicId=2trr62</t>
+  </si>
+  <si>
+    <t>A2WAVLJ0FU9UYQ</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1508wb-95-26090;topicId=2rc12o</t>
+  </si>
+  <si>
+    <t>A1T1FK3P2N408U</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0012wb-47-18993;topicId=2rc12o</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1217wb-28-08856;topicId=2rc12o</t>
+  </si>
+  <si>
+    <t>A1WGEJVGY3DI13</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0013wb-12-04299;topicId=2rc12o</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1910wb-21-00175;topicId=2rc12o</t>
+  </si>
+  <si>
+    <t>A2LO2DX6H49IKW</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0112wb-60-08498;topicId=2rc12o</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0201wb-78-26666;topicId=2rc12o</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0201wb-91-07427;topicId=2rc12o</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0915wb-33-22983;topicId=2rc12o</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0601wb-42-08172;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0202wb-51-05211;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>A1RU9BQLDZ1DSY</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1414wb-82-20474;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1904wb-26-11149;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1503wb-64-16315;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0103wb-58-26754;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1514wb-98-09364;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1306wb-06-13293;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>A3CLGUZHWU3699</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0310wb-07-15439;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>AKATSYE8XLYNL</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0302wb-75-33133;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-1402wb-12-13666;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0108wb-85-03300;topicId=3gwhon</t>
+  </si>
+  <si>
+    <t>AR50UBGSH10FJ</t>
+  </si>
+  <si>
+    <t>http://clef2017pool.ielab.webfactional.com/?doc=clueweb12-0915wb-67-24640;topicId=3gwhon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,6 +410,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -221,8 +440,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -238,7 +484,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -248,6 +494,33 @@
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -891,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -987,8 +1260,356 @@
         <v>48</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>89</v>
+      </c>
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>79</v>
+      </c>
+      <c r="B69" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>